<commit_message>
some changes, everything works besides subi
</commit_message>
<xml_diff>
--- a/SS.xlsx
+++ b/SS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\1BYTE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15114EC9-8C21-4A23-8097-C694F50E9595}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1245C615-8F2E-4C94-B4EB-E6482B3C5634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C3DBF6C8-52D7-45D1-B049-808B0AB7B082}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>ASM</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Move val into R</t>
+  </si>
+  <si>
+    <t>Implemented</t>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8750437-6B07-490F-A738-3C95E55B862D}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,9 +506,10 @@
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -524,157 +528,199 @@
       <c r="F1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="F9">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="H1:H10">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>